<commit_message>
Update the code - Add the mean_abundance
</commit_message>
<xml_diff>
--- a/input/vaginal_mrs.xlsx
+++ b/input/vaginal_mrs.xlsx
@@ -1931,1925 +1931,1925 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>20221229_BC05</t>
+          <t>20230328_BC49</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.0001436887058596133</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.006809120875666342</v>
+        <v>0.4734714817043348</v>
       </c>
       <c r="D41" t="n">
-        <v>0.02514169713097846</v>
+        <v>0.2367758489022886</v>
       </c>
       <c r="E41" t="n">
-        <v>0.02956382631082029</v>
+        <v>0.03461341248054982</v>
       </c>
       <c r="F41" t="n">
-        <v>0.08362274592650137</v>
+        <v>-0.06627049737934505</v>
       </c>
       <c r="G41" t="n">
-        <v>0.004259878554775546</v>
+        <v>0.405222155164785</v>
       </c>
       <c r="H41" t="n">
-        <v>-0.04841314364517252</v>
+        <v>-0.03138990012000637</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0004310661175788398</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0.06337060012279559</v>
+        <v>0.2128625484694311</v>
       </c>
       <c r="K41" t="n">
-        <v>0.005530279562489603</v>
+        <v>-0.01611671625890349</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>20221229_BC02</t>
+          <t>20230328_BC34</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>0.003242027769600459</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9073523165051274</v>
+        <v>-0.3055183303786462</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1645150926535315</v>
+        <v>-0.08975896611411276</v>
       </c>
       <c r="E42" t="n">
-        <v>0.02142998904424739</v>
+        <v>0.01563619740350616</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0006608411074830628</v>
+        <v>-0.02504774728019</v>
       </c>
       <c r="G42" t="n">
-        <v>0.4337580668915035</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.0001251219659195118</v>
+        <v>-0.05847624972055927</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>0.006675376245480656</v>
+        <v>0.1498593426501968</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.05360303970627268</v>
+        <v>-0.0642650581136136</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>20221229_BC07</t>
+          <t>20230328_BC36</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0003515090021242112</v>
+        <v>0.0002340432487577688</v>
       </c>
       <c r="C43" t="n">
-        <v>0.02070657309915077</v>
+        <v>0.3815807064938851</v>
       </c>
       <c r="D43" t="n">
-        <v>0.02277345523051209</v>
+        <v>-0.1978249993904991</v>
       </c>
       <c r="E43" t="n">
-        <v>0.02938209225055256</v>
+        <v>0.0005668567284404699</v>
       </c>
       <c r="F43" t="n">
-        <v>0.08574466944034755</v>
+        <v>-0.00037790906870502</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01418887026202229</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.003444643568369848</v>
+        <v>-0.00173854100843925</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>0.03257072340170612</v>
+        <v>0.005013971239921531</v>
       </c>
       <c r="K43" t="n">
-        <v>0.004713708404295343</v>
+        <v>-0.07387079684215367</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>20221229_BC04</t>
+          <t>20230328_BC32</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.0001083674969436144</v>
+        <v>0.09304865387277343</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6774008519921054</v>
+        <v>0.06807742493905188</v>
       </c>
       <c r="D44" t="n">
-        <v>0.333744987315867</v>
+        <v>0.01904300450032795</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0232582869225356</v>
+        <v>0.04326801355565556</v>
       </c>
       <c r="F44" t="n">
-        <v>0.002173060150725628</v>
+        <v>0.03099233014914076</v>
       </c>
       <c r="G44" t="n">
-        <v>0.4479313446485098</v>
+        <v>0.001312401093446732</v>
       </c>
       <c r="H44" t="n">
-        <v>-8.132125344261773e-05</v>
+        <v>-0.1089681114114057</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0.01612437489357143</v>
+        <v>0.3349538862559152</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.001871308369608463</v>
+        <v>0.02242734089608086</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>20221229_BC06</t>
+          <t>20230328_BC50</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.004732347989563723</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.05728468825514191</v>
+        <v>0.599542856884803</v>
       </c>
       <c r="D45" t="n">
-        <v>0.07704071163639019</v>
+        <v>0.3602220426005968</v>
       </c>
       <c r="E45" t="n">
-        <v>0.03991601464315513</v>
+        <v>0.0412572431457547</v>
       </c>
       <c r="F45" t="n">
-        <v>0.02272316899607529</v>
+        <v>-0.03214344749897289</v>
       </c>
       <c r="G45" t="n">
-        <v>0.04000247883859348</v>
+        <v>0.6299842377202385</v>
       </c>
       <c r="H45" t="n">
-        <v>-0.1755030642603472</v>
+        <v>-0.03469041747507113</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>0.455754082002866</v>
+        <v>0.1473185935807473</v>
       </c>
       <c r="K45" t="n">
-        <v>0.04103531872845018</v>
+        <v>0.01009839842068523</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>20230227_BC07</t>
+          <t>20230328_BC38</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.0007646094702336669</v>
+        <v>0.0005007129434112753</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.3582835190100669</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1604386497538714</v>
+        <v>0.2105141703694496</v>
       </c>
       <c r="E46" t="n">
-        <v>0.05357564501321219</v>
+        <v>0.03553814276429519</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.06466713108977493</v>
+        <v>-0.01444460447922911</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>0.0003768351015841419</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.1668373262989449</v>
+        <v>-0.07234279212903365</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>0.537458327250021</v>
+        <v>0.3275854741911098</v>
       </c>
       <c r="K46" t="n">
-        <v>0.05012886020817157</v>
+        <v>0.0141445630425926</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>20230227_BC08</t>
+          <t>20230328_BC56</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.0002462494751640889</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.3931005107260633</v>
+        <v>0.3994443391903282</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.1884938488984786</v>
+        <v>0.2002143629713586</v>
       </c>
       <c r="E47" t="n">
-        <v>0.01173239164674763</v>
+        <v>0.003053960828695146</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.0005400670468844388</v>
+        <v>-5.751579568346572e-05</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>0.000309812224699517</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.04130275202309252</v>
+        <v>-0.0006178647303781026</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0.07494473944002632</v>
+        <v>0.0163723632144271</v>
       </c>
       <c r="K47" t="n">
-        <v>-0.05921010167765459</v>
+        <v>-0.000227546315732848</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC05</t>
+          <t>20230328_BC40</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.0007516627235206429</v>
+        <v>0.0001259887988451976</v>
       </c>
       <c r="C48" t="n">
-        <v>0.002431375943846321</v>
+        <v>-0.3983897609429662</v>
       </c>
       <c r="D48" t="n">
-        <v>0.167290913396781</v>
+        <v>-0.1995439304146367</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0584486412172475</v>
+        <v>0.0008430762712905687</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.1904573785617034</v>
+        <v>0.001615504135889955</v>
       </c>
       <c r="G48" t="n">
-        <v>0.002362092658060304</v>
+        <v>0.00141516323001678</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.06661655346863167</v>
+        <v>-0.000565475756808927</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>0.4234863355985217</v>
+        <v>0.003977040273632854</v>
       </c>
       <c r="K48" t="n">
-        <v>0.07057382742844523</v>
+        <v>-0.07419869639469365</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC02</t>
+          <t>20230328_BC46</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001781252832546947</v>
+        <v>0.0001806694327884162</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.3965682382373086</v>
+        <v>0.4297223318867707</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.1956095547619678</v>
+        <v>-0.1840462697536613</v>
       </c>
       <c r="E49" t="n">
-        <v>0.001534040700747923</v>
+        <v>0.00242700722454102</v>
       </c>
       <c r="F49" t="n">
-        <v>0.003103319152292319</v>
+        <v>0.0005343661507276878</v>
       </c>
       <c r="G49" t="n">
-        <v>0.001432428234580979</v>
+        <v>0.03777994047901675</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.0007649669725093023</v>
+        <v>-0.003962228858374002</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>0.006008401483458241</v>
+        <v>0.002076829775157875</v>
       </c>
       <c r="K49" t="n">
-        <v>-0.07391959897034961</v>
+        <v>-0.0739414252118215</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC03</t>
+          <t>20230328_BC39</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.00202358367917119</v>
+        <v>0.1154463489834404</v>
       </c>
       <c r="C50" t="n">
-        <v>0.5641045363008861</v>
+        <v>0.001096478202762636</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2252554387906617</v>
+        <v>0.009573111895565417</v>
       </c>
       <c r="E50" t="n">
-        <v>0.04043734058626419</v>
+        <v>0.04367250421021832</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.03461410909283938</v>
+        <v>-0.001253003118877752</v>
       </c>
       <c r="G50" t="n">
-        <v>0.431269310956221</v>
+        <v>0.0003437291010828508</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.03460242536108083</v>
+        <v>-0.1509944902386528</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>0.2249651484635211</v>
+        <v>0.3204712196277874</v>
       </c>
       <c r="K50" t="n">
-        <v>0.002800715477050127</v>
+        <v>0.009784075835095878</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC10</t>
+          <t>20230328_BC55</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.3955749949190014</v>
+        <v>-0.3957196886854581</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.1976109848077313</v>
+        <v>-0.1992174067054509</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0005796516545710772</v>
+        <v>0.0002355827429344371</v>
       </c>
       <c r="F51" t="n">
-        <v>-3.327171235515791e-06</v>
+        <v>0.0005309146145305087</v>
       </c>
       <c r="G51" t="n">
-        <v>0.00168635246023749</v>
+        <v>0.00035476969375929</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>-0.003242859427732992</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>0.004063030136549752</v>
+        <v>0.001614584127191518</v>
       </c>
       <c r="K51" t="n">
-        <v>-0.0739292558085282</v>
+        <v>-0.07409770364425095</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC07</t>
+          <t>20230328_BC37</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.001720038275192313</v>
+        <v>0.0002018700335050141</v>
       </c>
       <c r="C52" t="n">
-        <v>0.06363508834757217</v>
+        <v>0.6444063348965056</v>
       </c>
       <c r="D52" t="n">
-        <v>0.03388231272059633</v>
+        <v>0.1923901183158563</v>
       </c>
       <c r="E52" t="n">
-        <v>0.02308410362769227</v>
+        <v>0.04362778695403654</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.0001256424861763877</v>
+        <v>0.001692343325596965</v>
       </c>
       <c r="G52" t="n">
-        <v>0.4551593729400856</v>
+        <v>0.8023676594734058</v>
       </c>
       <c r="H52" t="n">
-        <v>-0.0002360041662053635</v>
+        <v>-0.0009046411744440336</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>0.005891497190374688</v>
+        <v>0.0570425870118039</v>
       </c>
       <c r="K52" t="n">
-        <v>-0.0570442080358546</v>
+        <v>-0.04801326472917215</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC11</t>
+          <t>20230328_BC52</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.001957558868288111</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.002226147616308051</v>
+        <v>0.2613338714237741</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1051989447989606</v>
+        <v>-0.1675843979287207</v>
       </c>
       <c r="E53" t="n">
-        <v>0.04035558673171258</v>
+        <v>0.006814577840159208</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.1239008701492063</v>
+        <v>0.001590482118348704</v>
       </c>
       <c r="G53" t="n">
-        <v>0.003850106634696882</v>
+        <v>0.07472850348686792</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.1803340268049415</v>
+        <v>-0.01101803859812299</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>0.3263301820015905</v>
+        <v>0.03162223332087603</v>
       </c>
       <c r="K53" t="n">
-        <v>0.06307213783363309</v>
+        <v>-0.07257731563583986</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC01</t>
+          <t>20230328_BC53</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.03611284804440207</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.02637653436105057</v>
+        <v>0.3480025442825344</v>
       </c>
       <c r="D54" t="n">
-        <v>0.008534447192460697</v>
+        <v>-0.1934535125318542</v>
       </c>
       <c r="E54" t="n">
-        <v>0.03520654611182204</v>
+        <v>0.003188068091590521</v>
       </c>
       <c r="F54" t="n">
-        <v>0.005778279507964328</v>
+        <v>0.002904600243471131</v>
       </c>
       <c r="G54" t="n">
-        <v>0.01430495978994945</v>
+        <v>0.01270200713055006</v>
       </c>
       <c r="H54" t="n">
-        <v>-0.2868010864950036</v>
+        <v>-0.003751061464202092</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>0.2945679672334278</v>
+        <v>0.01319354670463498</v>
       </c>
       <c r="K54" t="n">
-        <v>0.01312985809421407</v>
+        <v>-0.07409659481279253</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC04</t>
+          <t>20230328_BC35</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.0006713675252128478</v>
+        <v>0.04961142045900987</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3997218760819036</v>
+        <v>0.00521900605442657</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.1978455978394082</v>
+        <v>-0.03030455920622626</v>
       </c>
       <c r="E55" t="n">
-        <v>0.001063917224430386</v>
+        <v>0.03428844518603862</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0003267453224374919</v>
+        <v>0.08254731748980279</v>
       </c>
       <c r="G55" t="n">
-        <v>0.001205448382074343</v>
+        <v>0.00208613048860985</v>
       </c>
       <c r="H55" t="n">
-        <v>-0.001000380974857434</v>
+        <v>-0.08617920515860394</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>0.003234855303132942</v>
+        <v>0.3453831580341765</v>
       </c>
       <c r="K55" t="n">
-        <v>-0.07398031752322884</v>
+        <v>-0.01538845856351616</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC06</t>
+          <t>20230328_BC44</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0002644620240375748</v>
+        <v>0.0008607191975030398</v>
       </c>
       <c r="C56" t="n">
-        <v>0.6668522803353798</v>
+        <v>0.3982977124970158</v>
       </c>
       <c r="D56" t="n">
-        <v>0.3173842983266412</v>
+        <v>-0.1923549108087214</v>
       </c>
       <c r="E56" t="n">
-        <v>0.02297244027443103</v>
+        <v>0.005256361543136298</v>
       </c>
       <c r="F56" t="n">
-        <v>-0.0002194665714951181</v>
+        <v>-0.001824722585110354</v>
       </c>
       <c r="G56" t="n">
-        <v>0.4647165114701988</v>
+        <v>0.0009745631715955816</v>
       </c>
       <c r="H56" t="n">
-        <v>-0.0003966930360563622</v>
+        <v>-0.04099566325857641</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>0.003016142899326173</v>
+        <v>0.02449763176891431</v>
       </c>
       <c r="K56" t="n">
-        <v>-0.006285478067598878</v>
+        <v>-0.06987807766289345</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>20230215_BC08</t>
+          <t>20230328_BC42</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.000874677648181117</v>
+        <v>0.004335913778937655</v>
       </c>
       <c r="C57" t="n">
-        <v>0.6607669630310343</v>
+        <v>0.002088621066367305</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1525008840123738</v>
+        <v>-0.08759632199366532</v>
       </c>
       <c r="E57" t="n">
-        <v>0.02526157837597555</v>
+        <v>0.07202300690066152</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0001219798136466278</v>
+        <v>0.1219805963843645</v>
       </c>
       <c r="G57" t="n">
-        <v>0.4807035510890998</v>
+        <v>0.001308322086717353</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.02118757719097042</v>
+        <v>-0.01505293590549694</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>0.02201613105549413</v>
+        <v>0.424794654996318</v>
       </c>
       <c r="K57" t="n">
-        <v>-0.05360255875489292</v>
+        <v>-0.04986328666780647</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC49</t>
+          <t>20230328_BC43</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>0.04360489125221342</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4734714817043348</v>
+        <v>0.004035841735210067</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2367758489022886</v>
+        <v>0.06173171734080975</v>
       </c>
       <c r="E58" t="n">
-        <v>0.03461341248054982</v>
+        <v>0.05205639607142023</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.06627049737934505</v>
+        <v>0.02769907979125615</v>
       </c>
       <c r="G58" t="n">
-        <v>0.405222155164785</v>
+        <v>0.001959263201339136</v>
       </c>
       <c r="H58" t="n">
-        <v>-0.03138990012000637</v>
+        <v>-0.03461377842243839</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>0.2128625484694311</v>
+        <v>0.2889378793093548</v>
       </c>
       <c r="K58" t="n">
-        <v>-0.01611671625890349</v>
+        <v>0.03909494746881032</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC34</t>
+          <t>20230328_BC47</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.003242027769600459</v>
+        <v>0.002925565762898168</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.3055183303786462</v>
+        <v>0.5250743423531566</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.08975896611411276</v>
+        <v>-0.1075265477378467</v>
       </c>
       <c r="E59" t="n">
-        <v>0.01563619740350616</v>
+        <v>0.02661626415265027</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.02504774728019</v>
+        <v>0.003702147873254721</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>0.1726275241549894</v>
       </c>
       <c r="H59" t="n">
-        <v>-0.05847624972055927</v>
+        <v>-0.02993349114000885</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>0.1498593426501968</v>
+        <v>0.08781089186231646</v>
       </c>
       <c r="K59" t="n">
-        <v>-0.0642650581136136</v>
+        <v>-0.0683812632474522</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC36</t>
+          <t>20230328_BC41</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0002340432487577688</v>
+        <v>0.001148637417649912</v>
       </c>
       <c r="C60" t="n">
-        <v>0.3815807064938851</v>
+        <v>0.7213107669487043</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.1978249993904991</v>
+        <v>0.4084712694191846</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0005668567284404699</v>
+        <v>0.03389207231252128</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.00037790906870502</v>
+        <v>-0.02181285141755355</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>0.5752444255527747</v>
       </c>
       <c r="H60" t="n">
-        <v>-0.00173854100843925</v>
+        <v>-0.03121150527249909</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>0.005013971239921531</v>
+        <v>0.1183917037325343</v>
       </c>
       <c r="K60" t="n">
-        <v>-0.07387079684215367</v>
+        <v>-0.0001174233531782534</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC32</t>
+          <t>20230328_BC33</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.09304865387277343</v>
+        <v>0.0002943184400109342</v>
       </c>
       <c r="C61" t="n">
-        <v>0.06807742493905188</v>
+        <v>0.3809792779422981</v>
       </c>
       <c r="D61" t="n">
-        <v>0.01904300450032795</v>
+        <v>0.06035340739613961</v>
       </c>
       <c r="E61" t="n">
-        <v>0.04326801355565556</v>
+        <v>0.006146375233451682</v>
       </c>
       <c r="F61" t="n">
-        <v>0.03099233014914076</v>
+        <v>-0.0002233724440588878</v>
       </c>
       <c r="G61" t="n">
-        <v>0.001312401093446732</v>
+        <v>0.001645535127311687</v>
       </c>
       <c r="H61" t="n">
-        <v>-0.1089681114114057</v>
+        <v>-0.00196282619532578</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>0.3349538862559152</v>
+        <v>0.07074068026922395</v>
       </c>
       <c r="K61" t="n">
-        <v>0.02242734089608086</v>
+        <v>-0.04913896965747732</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC50</t>
+          <t>20230328_BC51</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>0.0001660872515703498</v>
       </c>
       <c r="C62" t="n">
-        <v>0.599542856884803</v>
+        <v>0.4061654044813175</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3602220426005968</v>
+        <v>-0.1970753044955014</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0412572431457547</v>
+        <v>0.0006493603258158104</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.03214344749897289</v>
+        <v>0.0007005257599454669</v>
       </c>
       <c r="G62" t="n">
-        <v>0.6299842377202385</v>
+        <v>0.005474723952584086</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.03469041747507113</v>
+        <v>-0.002461028807268576</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>0.1473185935807473</v>
+        <v>0.003385590539910413</v>
       </c>
       <c r="K62" t="n">
-        <v>0.01009839842068523</v>
+        <v>-0.07391170681891351</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC38</t>
+          <t>20230328_BC54</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.0005007129434112753</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3582835190100669</v>
+        <v>0.2497498330109085</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2105141703694496</v>
+        <v>-0.108064479692432</v>
       </c>
       <c r="E63" t="n">
-        <v>0.03553814276429519</v>
+        <v>0.01151681891871075</v>
       </c>
       <c r="F63" t="n">
-        <v>-0.01444460447922911</v>
+        <v>9.428185745657239e-05</v>
       </c>
       <c r="G63" t="n">
-        <v>0.0003768351015841419</v>
+        <v>0.2216295086061052</v>
       </c>
       <c r="H63" t="n">
-        <v>-0.07234279212903365</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>0.3275854741911098</v>
+        <v>0.01098680432613265</v>
       </c>
       <c r="K63" t="n">
-        <v>0.0141445630425926</v>
+        <v>-0.07307955902222539</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC56</t>
+          <t>20230328_BC48</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>0.02053145260785224</v>
       </c>
       <c r="C64" t="n">
-        <v>0.3994443391903282</v>
+        <v>0.01013993207877523</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2002143629713586</v>
+        <v>-0.003052275376347325</v>
       </c>
       <c r="E64" t="n">
-        <v>0.003053960828695146</v>
+        <v>0.03898369620588998</v>
       </c>
       <c r="F64" t="n">
-        <v>-5.751579568346572e-05</v>
+        <v>0.006087165013871916</v>
       </c>
       <c r="G64" t="n">
-        <v>0.000309812224699517</v>
+        <v>0.003711011290748371</v>
       </c>
       <c r="H64" t="n">
-        <v>-0.0006178647303781026</v>
+        <v>-0.2119666022357595</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>0.0163723632144271</v>
+        <v>0.2665100180545621</v>
       </c>
       <c r="K64" t="n">
-        <v>-0.000227546315732848</v>
+        <v>-0.0024980311445477</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC40</t>
+          <t>20230328_BC45</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0001259887988451976</v>
+        <v>0.0002361391667761761</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.3983897609429662</v>
+        <v>-0.08864603235418382</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.1995439304146367</v>
+        <v>-0.1743894817776503</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0008430762712905687</v>
+        <v>0.01154451775673332</v>
       </c>
       <c r="F65" t="n">
-        <v>0.001615504135889955</v>
+        <v>0.003115222304964215</v>
       </c>
       <c r="G65" t="n">
-        <v>0.00141516323001678</v>
+        <v>0.05802032297637293</v>
       </c>
       <c r="H65" t="n">
-        <v>-0.000565475756808927</v>
+        <v>-0.00141167699072312</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>0.003977040273632854</v>
+        <v>0.09422268086451825</v>
       </c>
       <c r="K65" t="n">
-        <v>-0.07419869639469365</v>
+        <v>-0.0734192933009388</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC46</t>
+          <t>20221229_BC05</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.0001806694327884162</v>
+        <v>0.0001436887058596133</v>
       </c>
       <c r="C66" t="n">
-        <v>0.4297223318867707</v>
+        <v>0.006809120875666342</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.1840462697536613</v>
+        <v>0.02514169713097846</v>
       </c>
       <c r="E66" t="n">
-        <v>0.00242700722454102</v>
+        <v>0.02956382631082029</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0005343661507276878</v>
+        <v>0.08362274592650137</v>
       </c>
       <c r="G66" t="n">
-        <v>0.03777994047901675</v>
+        <v>0.004259878554775546</v>
       </c>
       <c r="H66" t="n">
-        <v>-0.003962228858374002</v>
+        <v>-0.04841314364517252</v>
       </c>
       <c r="I66" t="n">
-        <v>0</v>
+        <v>0.0004310661175788398</v>
       </c>
       <c r="J66" t="n">
-        <v>0.002076829775157875</v>
+        <v>0.06337060012279559</v>
       </c>
       <c r="K66" t="n">
-        <v>-0.0739414252118215</v>
+        <v>0.005530279562489603</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC39</t>
+          <t>20221229_BC02</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1154463489834404</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.001096478202762636</v>
+        <v>0.9073523165051274</v>
       </c>
       <c r="D67" t="n">
-        <v>0.009573111895565417</v>
+        <v>0.1645150926535315</v>
       </c>
       <c r="E67" t="n">
-        <v>0.04367250421021832</v>
+        <v>0.02142998904424739</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.001253003118877752</v>
+        <v>0.0006608411074830628</v>
       </c>
       <c r="G67" t="n">
-        <v>0.0003437291010828508</v>
+        <v>0.4337580668915035</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.1509944902386528</v>
+        <v>-0.0001251219659195118</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>0.3204712196277874</v>
+        <v>0.006675376245480656</v>
       </c>
       <c r="K67" t="n">
-        <v>0.009784075835095878</v>
+        <v>-0.05360303970627268</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC55</t>
+          <t>20221229_BC07</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>0.0003515090021242112</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.3957196886854581</v>
+        <v>0.02070657309915077</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.1992174067054509</v>
+        <v>0.02277345523051209</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0002355827429344371</v>
+        <v>0.02938209225055256</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0005309146145305087</v>
+        <v>0.08574466944034755</v>
       </c>
       <c r="G68" t="n">
-        <v>0.00035476969375929</v>
+        <v>0.01418887026202229</v>
       </c>
       <c r="H68" t="n">
-        <v>-0.003242859427732992</v>
+        <v>-0.003444643568369848</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>0.001614584127191518</v>
+        <v>0.03257072340170612</v>
       </c>
       <c r="K68" t="n">
-        <v>-0.07409770364425095</v>
+        <v>0.004713708404295343</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC37</t>
+          <t>20221229_BC04</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0002018700335050141</v>
+        <v>0.0001083674969436144</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6444063348965056</v>
+        <v>0.6774008519921054</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1923901183158563</v>
+        <v>0.333744987315867</v>
       </c>
       <c r="E69" t="n">
-        <v>0.04362778695403654</v>
+        <v>0.0232582869225356</v>
       </c>
       <c r="F69" t="n">
-        <v>0.001692343325596965</v>
+        <v>0.002173060150725628</v>
       </c>
       <c r="G69" t="n">
-        <v>0.8023676594734058</v>
+        <v>0.4479313446485098</v>
       </c>
       <c r="H69" t="n">
-        <v>-0.0009046411744440336</v>
+        <v>-8.132125344261773e-05</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>0.0570425870118039</v>
+        <v>0.01612437489357143</v>
       </c>
       <c r="K69" t="n">
-        <v>-0.04801326472917215</v>
+        <v>-0.001871308369608463</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC52</t>
+          <t>20221229_BC06</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>0.004732347989563723</v>
       </c>
       <c r="C70" t="n">
-        <v>0.2613338714237741</v>
+        <v>0.05728468825514191</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.1675843979287207</v>
+        <v>0.07704071163639019</v>
       </c>
       <c r="E70" t="n">
-        <v>0.006814577840159208</v>
+        <v>0.03991601464315513</v>
       </c>
       <c r="F70" t="n">
-        <v>0.001590482118348704</v>
+        <v>0.02272316899607529</v>
       </c>
       <c r="G70" t="n">
-        <v>0.07472850348686792</v>
+        <v>0.04000247883859348</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.01101803859812299</v>
+        <v>-0.1755030642603472</v>
       </c>
       <c r="I70" t="n">
         <v>0</v>
       </c>
       <c r="J70" t="n">
-        <v>0.03162223332087603</v>
+        <v>0.455754082002866</v>
       </c>
       <c r="K70" t="n">
-        <v>-0.07257731563583986</v>
+        <v>0.04103531872845018</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC53</t>
+          <t>20230227_BC07</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>0.0007646094702336669</v>
       </c>
       <c r="C71" t="n">
-        <v>0.3480025442825344</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>-0.1934535125318542</v>
+        <v>0.1604386497538714</v>
       </c>
       <c r="E71" t="n">
-        <v>0.003188068091590521</v>
+        <v>0.05357564501321219</v>
       </c>
       <c r="F71" t="n">
-        <v>0.002904600243471131</v>
+        <v>-0.06466713108977493</v>
       </c>
       <c r="G71" t="n">
-        <v>0.01270200713055006</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>-0.003751061464202092</v>
+        <v>-0.1668373262989449</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>0.01319354670463498</v>
+        <v>0.537458327250021</v>
       </c>
       <c r="K71" t="n">
-        <v>-0.07409659481279253</v>
+        <v>0.05012886020817157</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC35</t>
+          <t>20230227_BC08</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.04961142045900987</v>
+        <v>0.0002462494751640889</v>
       </c>
       <c r="C72" t="n">
-        <v>0.00521900605442657</v>
+        <v>-0.3931005107260633</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.03030455920622626</v>
+        <v>-0.1884938488984786</v>
       </c>
       <c r="E72" t="n">
-        <v>0.03428844518603862</v>
+        <v>0.01173239164674763</v>
       </c>
       <c r="F72" t="n">
-        <v>0.08254731748980279</v>
+        <v>-0.0005400670468844388</v>
       </c>
       <c r="G72" t="n">
-        <v>0.00208613048860985</v>
+        <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>-0.08617920515860394</v>
+        <v>-0.04130275202309252</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
       </c>
       <c r="J72" t="n">
-        <v>0.3453831580341765</v>
+        <v>0.07494473944002632</v>
       </c>
       <c r="K72" t="n">
-        <v>-0.01538845856351616</v>
+        <v>-0.05921010167765459</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC44</t>
+          <t>20230322_BC72</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.0008607191975030398</v>
+        <v>0.0005957349376948467</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3982977124970158</v>
+        <v>0.3266341149358714</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.1923549108087214</v>
+        <v>-0.1967936468330777</v>
       </c>
       <c r="E73" t="n">
-        <v>0.005256361543136298</v>
+        <v>0.0006879170818814007</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.001824722585110354</v>
+        <v>0.0008564011504021497</v>
       </c>
       <c r="G73" t="n">
-        <v>0.0009745631715955816</v>
+        <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>-0.04099566325857641</v>
+        <v>0</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>0.02449763176891431</v>
+        <v>0.006222209588455295</v>
       </c>
       <c r="K73" t="n">
-        <v>-0.06987807766289345</v>
+        <v>-0.07358326332373645</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC42</t>
+          <t>20230322_BC77</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.004335913778937655</v>
+        <v>0.00470366355490682</v>
       </c>
       <c r="C74" t="n">
-        <v>0.002088621066367305</v>
+        <v>0.3224087571479483</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.08759632199366532</v>
+        <v>0.1200129272720805</v>
       </c>
       <c r="E74" t="n">
-        <v>0.07202300690066152</v>
+        <v>0.005685359355822619</v>
       </c>
       <c r="F74" t="n">
-        <v>0.1219805963843645</v>
+        <v>0.002312787483989106</v>
       </c>
       <c r="G74" t="n">
-        <v>0.001308322086717353</v>
+        <v>0.0004999254641340411</v>
       </c>
       <c r="H74" t="n">
-        <v>-0.01505293590549694</v>
+        <v>-0.01117159670343016</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>0.424794654996318</v>
+        <v>0.0233251146188738</v>
       </c>
       <c r="K74" t="n">
-        <v>-0.04986328666780647</v>
+        <v>-0.01660256829037488</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC43</t>
+          <t>20230322_BC89</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.04360489125221342</v>
+        <v>0.0004047578036891061</v>
       </c>
       <c r="C75" t="n">
-        <v>0.004035841735210067</v>
+        <v>0.2979716544032026</v>
       </c>
       <c r="D75" t="n">
-        <v>0.06173171734080975</v>
+        <v>-0.1435404476265331</v>
       </c>
       <c r="E75" t="n">
-        <v>0.05205639607142023</v>
+        <v>0.02425899510943187</v>
       </c>
       <c r="F75" t="n">
-        <v>0.02769907979125615</v>
+        <v>0.003094762268407197</v>
       </c>
       <c r="G75" t="n">
-        <v>0.001959263201339136</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>-0.03461377842243839</v>
+        <v>-0.00180634262519586</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>0.2889378793093548</v>
+        <v>0.283731721222013</v>
       </c>
       <c r="K75" t="n">
-        <v>0.03909494746881032</v>
+        <v>-0.05466572447187669</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC47</t>
+          <t>20230322_BC73</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.002925565762898168</v>
+        <v>0.0003774950209381719</v>
       </c>
       <c r="C76" t="n">
-        <v>0.5250743423531566</v>
+        <v>0.001360310974638831</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.1075265477378467</v>
+        <v>0.1532091752974166</v>
       </c>
       <c r="E76" t="n">
-        <v>0.02661626415265027</v>
+        <v>0.0711303332508099</v>
       </c>
       <c r="F76" t="n">
-        <v>0.003702147873254721</v>
+        <v>-0.05671926542422598</v>
       </c>
       <c r="G76" t="n">
-        <v>0.1726275241549894</v>
+        <v>0.0004255124605938259</v>
       </c>
       <c r="H76" t="n">
-        <v>-0.02993349114000885</v>
+        <v>-0.03677417963493045</v>
       </c>
       <c r="I76" t="n">
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>0.08781089186231646</v>
+        <v>0.5587231085931922</v>
       </c>
       <c r="K76" t="n">
-        <v>-0.0683812632474522</v>
+        <v>0.05967478774968606</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC41</t>
+          <t>20230322_BC74</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.001148637417649912</v>
+        <v>0.0002050786870548268</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7213107669487043</v>
+        <v>0.7866420849621016</v>
       </c>
       <c r="D77" t="n">
-        <v>0.4084712694191846</v>
+        <v>0.3030157815907856</v>
       </c>
       <c r="E77" t="n">
-        <v>0.03389207231252128</v>
+        <v>0.04160919023925777</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.02181285141755355</v>
+        <v>0.007159346532333234</v>
       </c>
       <c r="G77" t="n">
-        <v>0.5752444255527747</v>
+        <v>0.7260773203249894</v>
       </c>
       <c r="H77" t="n">
-        <v>-0.03121150527249909</v>
+        <v>-0.007631127057487481</v>
       </c>
       <c r="I77" t="n">
         <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>0.1183917037325343</v>
+        <v>0.09878366251778299</v>
       </c>
       <c r="K77" t="n">
-        <v>-0.0001174233531782534</v>
+        <v>-0.02563966161033644</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC33</t>
+          <t>20230322_BC75</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.0002943184400109342</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.3809792779422981</v>
+        <v>-0.01585101907006612</v>
       </c>
       <c r="D78" t="n">
-        <v>0.06035340739613961</v>
+        <v>-0.1964023562735602</v>
       </c>
       <c r="E78" t="n">
-        <v>0.006146375233451682</v>
+        <v>0.003106612292561146</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.0002233724440588878</v>
+        <v>0.0003329371532924941</v>
       </c>
       <c r="G78" t="n">
-        <v>0.001645535127311687</v>
+        <v>0.002142976721455944</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.00196282619532578</v>
+        <v>-0.002777550374411077</v>
       </c>
       <c r="I78" t="n">
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>0.07074068026922395</v>
+        <v>0.02410709313842841</v>
       </c>
       <c r="K78" t="n">
-        <v>-0.04913896965747732</v>
+        <v>-0.07032824245064531</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC51</t>
+          <t>20230322_BC76</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.0001660872515703498</v>
+        <v>0.0003750451586889561</v>
       </c>
       <c r="C79" t="n">
-        <v>0.4061654044813175</v>
+        <v>0.4332033026983651</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.1970753044955014</v>
+        <v>-0.1787125979886822</v>
       </c>
       <c r="E79" t="n">
-        <v>0.0006493603258158104</v>
+        <v>0.004453606566888041</v>
       </c>
       <c r="F79" t="n">
-        <v>0.0007005257599454669</v>
+        <v>-0.0002742354187623928</v>
       </c>
       <c r="G79" t="n">
-        <v>0.005474723952584086</v>
+        <v>0.04226783572174848</v>
       </c>
       <c r="H79" t="n">
-        <v>-0.002461028807268576</v>
+        <v>0</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>0.003385590539910413</v>
+        <v>0.02784455675744881</v>
       </c>
       <c r="K79" t="n">
-        <v>-0.07391170681891351</v>
+        <v>-0.07394310855212725</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC54</t>
+          <t>20230322_BC96</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>0.0005777345143148615</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2497498330109085</v>
+        <v>0.4148077457482883</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.108064479692432</v>
+        <v>-0.1871570575900215</v>
       </c>
       <c r="E80" t="n">
-        <v>0.01151681891871075</v>
+        <v>0.005353380527920511</v>
       </c>
       <c r="F80" t="n">
-        <v>9.428185745657239e-05</v>
+        <v>-9.493152118558392e-05</v>
       </c>
       <c r="G80" t="n">
-        <v>0.2216295086061052</v>
+        <v>0.02018333166142914</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>-0.0181434029254432</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>0.01098680432613265</v>
+        <v>0.0279664888000852</v>
       </c>
       <c r="K80" t="n">
-        <v>-0.07307955902222539</v>
+        <v>-0.06988218092605747</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC48</t>
+          <t>20230322_BC79</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.02053145260785224</v>
+        <v>0.001595805326623886</v>
       </c>
       <c r="C81" t="n">
-        <v>0.01013993207877523</v>
+        <v>0.0003208562489406237</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.003052275376347325</v>
+        <v>0.1066224305048903</v>
       </c>
       <c r="E81" t="n">
-        <v>0.03898369620588998</v>
+        <v>0.055263236796379</v>
       </c>
       <c r="F81" t="n">
-        <v>0.006087165013871916</v>
+        <v>-0.02675364813148197</v>
       </c>
       <c r="G81" t="n">
-        <v>0.003711011290748371</v>
+        <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>-0.2119666022357595</v>
+        <v>-0.06750474379283376</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>0.2665100180545621</v>
+        <v>0.3242803035519092</v>
       </c>
       <c r="K81" t="n">
-        <v>-0.0024980311445477</v>
+        <v>0.05135114727595195</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>20230328_BC45</t>
+          <t>20230322_BC71</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.0002361391667761761</v>
+        <v>0.1436741946998149</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.08864603235418382</v>
+        <v>-0.0002044413135630802</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.1743894817776503</v>
+        <v>0.001986327905227178</v>
       </c>
       <c r="E82" t="n">
-        <v>0.01154451775673332</v>
+        <v>0.003388561787408536</v>
       </c>
       <c r="F82" t="n">
-        <v>0.003115222304964215</v>
+        <v>0.07570906212642746</v>
       </c>
       <c r="G82" t="n">
-        <v>0.05802032297637293</v>
+        <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.00141167699072312</v>
+        <v>0</v>
       </c>
       <c r="I82" t="n">
         <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>0.09422268086451825</v>
+        <v>0.01513288341148863</v>
       </c>
       <c r="K82" t="n">
-        <v>-0.0734192933009388</v>
+        <v>0.0004847669301326959</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC72</t>
+          <t>20230215_BC05</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.0005957349376948467</v>
+        <v>0.0007516627235206429</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3266341149358714</v>
+        <v>0.002431375943846321</v>
       </c>
       <c r="D83" t="n">
-        <v>-0.1967936468330777</v>
+        <v>0.167290913396781</v>
       </c>
       <c r="E83" t="n">
-        <v>0.0006879170818814007</v>
+        <v>0.0584486412172475</v>
       </c>
       <c r="F83" t="n">
-        <v>0.0008564011504021497</v>
+        <v>-0.1904573785617034</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>0.002362092658060304</v>
       </c>
       <c r="H83" t="n">
-        <v>0</v>
+        <v>-0.06661655346863167</v>
       </c>
       <c r="I83" t="n">
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>0.006222209588455295</v>
+        <v>0.4234863355985217</v>
       </c>
       <c r="K83" t="n">
-        <v>-0.07358326332373645</v>
+        <v>0.07057382742844523</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC77</t>
+          <t>20230215_BC02</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.00470366355490682</v>
+        <v>0.001781252832546947</v>
       </c>
       <c r="C84" t="n">
-        <v>0.3224087571479483</v>
+        <v>-0.3965682382373086</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1200129272720805</v>
+        <v>-0.1956095547619678</v>
       </c>
       <c r="E84" t="n">
-        <v>0.005685359355822619</v>
+        <v>0.001534040700747923</v>
       </c>
       <c r="F84" t="n">
-        <v>0.002312787483989106</v>
+        <v>0.003103319152292319</v>
       </c>
       <c r="G84" t="n">
-        <v>0.0004999254641340411</v>
+        <v>0.001432428234580979</v>
       </c>
       <c r="H84" t="n">
-        <v>-0.01117159670343016</v>
+        <v>-0.0007649669725093023</v>
       </c>
       <c r="I84" t="n">
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>0.0233251146188738</v>
+        <v>0.006008401483458241</v>
       </c>
       <c r="K84" t="n">
-        <v>-0.01660256829037488</v>
+        <v>-0.07391959897034961</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC89</t>
+          <t>20230215_BC03</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0004047578036891061</v>
+        <v>0.00202358367917119</v>
       </c>
       <c r="C85" t="n">
-        <v>0.2979716544032026</v>
+        <v>0.5641045363008861</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.1435404476265331</v>
+        <v>0.2252554387906617</v>
       </c>
       <c r="E85" t="n">
-        <v>0.02425899510943187</v>
+        <v>0.04043734058626419</v>
       </c>
       <c r="F85" t="n">
-        <v>0.003094762268407197</v>
+        <v>-0.03461410909283938</v>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>0.431269310956221</v>
       </c>
       <c r="H85" t="n">
-        <v>-0.00180634262519586</v>
+        <v>-0.03460242536108083</v>
       </c>
       <c r="I85" t="n">
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>0.283731721222013</v>
+        <v>0.2249651484635211</v>
       </c>
       <c r="K85" t="n">
-        <v>-0.05466572447187669</v>
+        <v>0.002800715477050127</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC73</t>
+          <t>20230215_BC10</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.0003774950209381719</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.001360310974638831</v>
+        <v>-0.3955749949190014</v>
       </c>
       <c r="D86" t="n">
-        <v>0.1532091752974166</v>
+        <v>-0.1976109848077313</v>
       </c>
       <c r="E86" t="n">
-        <v>0.0711303332508099</v>
+        <v>0.0005796516545710772</v>
       </c>
       <c r="F86" t="n">
-        <v>-0.05671926542422598</v>
+        <v>-3.327171235515791e-06</v>
       </c>
       <c r="G86" t="n">
-        <v>0.0004255124605938259</v>
+        <v>0.00168635246023749</v>
       </c>
       <c r="H86" t="n">
-        <v>-0.03677417963493045</v>
+        <v>0</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>0.5587231085931922</v>
+        <v>0.004063030136549752</v>
       </c>
       <c r="K86" t="n">
-        <v>0.05967478774968606</v>
+        <v>-0.0739292558085282</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC74</t>
+          <t>20230215_BC07</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.0002050786870548268</v>
+        <v>0.001720038275192313</v>
       </c>
       <c r="C87" t="n">
-        <v>0.7866420849621016</v>
+        <v>0.06363508834757217</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3030157815907856</v>
+        <v>0.03388231272059633</v>
       </c>
       <c r="E87" t="n">
-        <v>0.04160919023925777</v>
+        <v>0.02308410362769227</v>
       </c>
       <c r="F87" t="n">
-        <v>0.007159346532333234</v>
+        <v>-0.0001256424861763877</v>
       </c>
       <c r="G87" t="n">
-        <v>0.7260773203249894</v>
+        <v>0.4551593729400856</v>
       </c>
       <c r="H87" t="n">
-        <v>-0.007631127057487481</v>
+        <v>-0.0002360041662053635</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
       </c>
       <c r="J87" t="n">
-        <v>0.09878366251778299</v>
+        <v>0.005891497190374688</v>
       </c>
       <c r="K87" t="n">
-        <v>-0.02563966161033644</v>
+        <v>-0.0570442080358546</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC75</t>
+          <t>20230215_BC11</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>0.001957558868288111</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.01585101907006612</v>
+        <v>0.002226147616308051</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.1964023562735602</v>
+        <v>0.1051989447989606</v>
       </c>
       <c r="E88" t="n">
-        <v>0.003106612292561146</v>
+        <v>0.04035558673171258</v>
       </c>
       <c r="F88" t="n">
-        <v>0.0003329371532924941</v>
+        <v>-0.1239008701492063</v>
       </c>
       <c r="G88" t="n">
-        <v>0.002142976721455944</v>
+        <v>0.003850106634696882</v>
       </c>
       <c r="H88" t="n">
-        <v>-0.002777550374411077</v>
+        <v>-0.1803340268049415</v>
       </c>
       <c r="I88" t="n">
         <v>0</v>
       </c>
       <c r="J88" t="n">
-        <v>0.02410709313842841</v>
+        <v>0.3263301820015905</v>
       </c>
       <c r="K88" t="n">
-        <v>-0.07032824245064531</v>
+        <v>0.06307213783363309</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC76</t>
+          <t>20230215_BC01</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.0003750451586889561</v>
+        <v>0.03611284804440207</v>
       </c>
       <c r="C89" t="n">
-        <v>0.4332033026983651</v>
+        <v>0.02637653436105057</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.1787125979886822</v>
+        <v>0.008534447192460697</v>
       </c>
       <c r="E89" t="n">
-        <v>0.004453606566888041</v>
+        <v>0.03520654611182204</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.0002742354187623928</v>
+        <v>0.005778279507964328</v>
       </c>
       <c r="G89" t="n">
-        <v>0.04226783572174848</v>
+        <v>0.01430495978994945</v>
       </c>
       <c r="H89" t="n">
-        <v>0</v>
+        <v>-0.2868010864950036</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
       </c>
       <c r="J89" t="n">
-        <v>0.02784455675744881</v>
+        <v>0.2945679672334278</v>
       </c>
       <c r="K89" t="n">
-        <v>-0.07394310855212725</v>
+        <v>0.01312985809421407</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC96</t>
+          <t>20230215_BC04</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.0005777345143148615</v>
+        <v>0.0006713675252128478</v>
       </c>
       <c r="C90" t="n">
-        <v>0.4148077457482883</v>
+        <v>0.3997218760819036</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.1871570575900215</v>
+        <v>-0.1978455978394082</v>
       </c>
       <c r="E90" t="n">
-        <v>0.005353380527920511</v>
+        <v>0.001063917224430386</v>
       </c>
       <c r="F90" t="n">
-        <v>-9.493152118558392e-05</v>
+        <v>0.0003267453224374919</v>
       </c>
       <c r="G90" t="n">
-        <v>0.02018333166142914</v>
+        <v>0.001205448382074343</v>
       </c>
       <c r="H90" t="n">
-        <v>-0.0181434029254432</v>
+        <v>-0.001000380974857434</v>
       </c>
       <c r="I90" t="n">
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>0.0279664888000852</v>
+        <v>0.003234855303132942</v>
       </c>
       <c r="K90" t="n">
-        <v>-0.06988218092605747</v>
+        <v>-0.07398031752322884</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC79</t>
+          <t>20230215_BC06</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.001595805326623886</v>
+        <v>0.0002644620240375748</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0003208562489406237</v>
+        <v>0.6668522803353798</v>
       </c>
       <c r="D91" t="n">
-        <v>0.1066224305048903</v>
+        <v>0.3173842983266412</v>
       </c>
       <c r="E91" t="n">
-        <v>0.055263236796379</v>
+        <v>0.02297244027443103</v>
       </c>
       <c r="F91" t="n">
-        <v>-0.02675364813148197</v>
+        <v>-0.0002194665714951181</v>
       </c>
       <c r="G91" t="n">
-        <v>0</v>
+        <v>0.4647165114701988</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.06750474379283376</v>
+        <v>-0.0003966930360563622</v>
       </c>
       <c r="I91" t="n">
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>0.3242803035519092</v>
+        <v>0.003016142899326173</v>
       </c>
       <c r="K91" t="n">
-        <v>0.05135114727595195</v>
+        <v>-0.006285478067598878</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>20230322_BC71</t>
+          <t>20230215_BC08</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.1436741946998149</v>
+        <v>0.000874677648181117</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.0002044413135630802</v>
+        <v>0.6607669630310343</v>
       </c>
       <c r="D92" t="n">
-        <v>0.001986327905227178</v>
+        <v>0.1525008840123738</v>
       </c>
       <c r="E92" t="n">
-        <v>0.003388561787408536</v>
+        <v>0.02526157837597555</v>
       </c>
       <c r="F92" t="n">
-        <v>0.07570906212642746</v>
+        <v>0.0001219798136466278</v>
       </c>
       <c r="G92" t="n">
-        <v>0</v>
+        <v>0.4807035510890998</v>
       </c>
       <c r="H92" t="n">
-        <v>0</v>
+        <v>-0.02118757719097042</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
       </c>
       <c r="J92" t="n">
-        <v>0.01513288341148863</v>
+        <v>0.02201613105549413</v>
       </c>
       <c r="K92" t="n">
-        <v>0.0004847669301326959</v>
+        <v>-0.05360255875489292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>